<commit_message>
Notes for class on October 7, 2019
</commit_message>
<xml_diff>
--- a/Reference/Template_Framework_Monti_MakingCommunity_2019v00.xlsx
+++ b/Reference/Template_Framework_Monti_MakingCommunity_2019v00.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOC5800\Reference\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOC5060\Reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,12 +38,6 @@
     <t>Exclusive</t>
   </si>
   <si>
-    <t>Privacy Respected</t>
-  </si>
-  <si>
-    <t>Public Scrutiny</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
@@ -57,6 +51,12 @@
   </si>
   <si>
     <t>Total counts</t>
+  </si>
+  <si>
+    <t>Mild Punishment</t>
+  </si>
+  <si>
+    <t>Severe Punishment</t>
   </si>
 </sst>
 </file>
@@ -88,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -142,37 +142,6 @@
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -276,58 +245,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -340,43 +266,126 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="double">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="double">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="double">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="double">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="double">
+          <color auto="1"/>
+        </right>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -387,6 +396,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G32" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10">
+  <autoFilter ref="A2:G32">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Data" dataDxfId="7"/>
+    <tableColumn id="2" name="Inclusive" dataDxfId="6"/>
+    <tableColumn id="3" name="Exclusive" dataDxfId="5"/>
+    <tableColumn id="4" name="Loose Adherence" dataDxfId="4"/>
+    <tableColumn id="5" name="Strict Adherence" dataDxfId="3"/>
+    <tableColumn id="6" name="Mild Punishment" dataDxfId="2"/>
+    <tableColumn id="7" name="Severe Punishment" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -695,285 +728,343 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="100.7109375" customWidth="1"/>
-    <col min="2" max="7" width="10.7109375" style="7" customWidth="1"/>
+    <col min="2" max="7" width="12.7109375" style="5" customWidth="1"/>
     <col min="8" max="9" width="10.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="14"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="14"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="9"/>
-    </row>
-    <row r="33" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="13">
+      <c r="B33" s="16">
         <f>COUNTA(B$3:B$32)</f>
         <v>0</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="17">
         <f t="shared" ref="C33:G33" si="0">COUNTA(C$3:C$32)</f>
         <v>0</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -987,5 +1078,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>